<commit_message>
DA 16 | Day 3
</commit_message>
<xml_diff>
--- a/Batch/16/Curriculum/Day_3_Arithmetic.xlsx
+++ b/Batch/16/Curriculum/Day_3_Arithmetic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28422"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\15\Curriculum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\16\Curriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D50E60-3A80-46F7-9566-6F14857CEA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5885644-2DC4-47DB-9D21-3D295A2DAD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goal" sheetId="1" r:id="rId1"/>
@@ -680,7 +680,9 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -691,19 +693,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -723,8 +725,6 @@
     <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +748,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10990</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>127488</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2962275" cy="1609725"/>
     <xdr:pic>
@@ -772,6 +772,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6795721" y="677007"/>
+          <a:ext cx="2962275" cy="1609725"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1346,57 +1350,57 @@
   <sheetData>
     <row r="1" spans="3:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="3" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
     </row>
     <row r="5" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="36"/>
     </row>
     <row r="6" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="7" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="39"/>
     </row>
     <row r="8" spans="3:16" ht="12" customHeight="1" x14ac:dyDescent="0.7">
       <c r="C8" s="1"/>
@@ -1404,495 +1408,495 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="28"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="30"/>
     </row>
     <row r="10" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="33"/>
     </row>
     <row r="11" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="33"/>
     </row>
     <row r="12" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="33"/>
     </row>
     <row r="13" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="36"/>
     </row>
     <row r="14" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="15" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="39"/>
     </row>
     <row r="16" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="17" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
     </row>
     <row r="18" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
     </row>
     <row r="19" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>2</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="39"/>
     </row>
     <row r="20" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>3</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
     </row>
     <row r="21" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>4</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
     </row>
     <row r="22" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C22" s="3">
         <v>5</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
     </row>
     <row r="23" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C23" s="3">
         <v>6</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C24" s="3">
         <v>7</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C25" s="3">
         <v>8</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="39"/>
     </row>
     <row r="26" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C26" s="3">
         <v>9</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="39"/>
     </row>
     <row r="27" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C27" s="3">
         <v>10</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="39"/>
     </row>
     <row r="28" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C28" s="3">
         <v>11</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="39"/>
     </row>
     <row r="29" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C29" s="3">
         <v>12</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="39"/>
     </row>
     <row r="30" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C30" s="3">
         <v>13</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="39"/>
     </row>
     <row r="31" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C31" s="3">
         <v>14</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="39"/>
     </row>
     <row r="32" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C32" s="3">
         <v>15</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="39"/>
     </row>
     <row r="33" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C33" s="3">
         <v>16</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="39"/>
     </row>
     <row r="34" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C34" s="3">
         <v>17</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="39"/>
     </row>
     <row r="35" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C35" s="3">
         <v>18</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="39"/>
     </row>
     <row r="36" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C36" s="3">
         <v>19</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="39"/>
     </row>
     <row r="37" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C37" s="3">
         <v>20</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="39"/>
     </row>
     <row r="38" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C38" s="3">
         <v>21</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="39"/>
     </row>
     <row r="39" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="40" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="41" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="37"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="39"/>
     </row>
     <row r="42" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="43" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="28"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="30"/>
     </row>
     <row r="44" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C44" s="29"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
-      <c r="O44" s="30"/>
-      <c r="P44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="32"/>
+      <c r="P44" s="33"/>
     </row>
     <row r="45" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C45" s="29"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30"/>
-      <c r="O45" s="30"/>
-      <c r="P45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="33"/>
     </row>
     <row r="46" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C46" s="29"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
-      <c r="O46" s="30"/>
-      <c r="P46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="33"/>
     </row>
     <row r="47" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C47" s="32"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="33"/>
-      <c r="N47" s="33"/>
-      <c r="O47" s="33"/>
-      <c r="P47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="35"/>
+      <c r="N47" s="35"/>
+      <c r="O47" s="35"/>
+      <c r="P47" s="36"/>
     </row>
     <row r="48" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2849,21 +2853,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="G2:L5"/>
-    <mergeCell ref="C7:P7"/>
-    <mergeCell ref="C9:P13"/>
-    <mergeCell ref="C15:P15"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="D18:I18"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="D20:I20"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="D34:I34"/>
     <mergeCell ref="C43:P47"/>
     <mergeCell ref="D27:I27"/>
     <mergeCell ref="D28:I28"/>
@@ -2877,6 +2866,21 @@
     <mergeCell ref="D37:I37"/>
     <mergeCell ref="D38:I38"/>
     <mergeCell ref="C41:P41"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D34:I34"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="D20:I20"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="G2:L5"/>
+    <mergeCell ref="C7:P7"/>
+    <mergeCell ref="C9:P13"/>
+    <mergeCell ref="C15:P15"/>
+    <mergeCell ref="D17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2897,14 +2901,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="32"/>
-      <c r="H2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2981,26 +2985,26 @@
       <c r="C15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="37"/>
+      <c r="E15" s="39"/>
     </row>
     <row r="16" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="18"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="37"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="18"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="39"/>
     </row>
     <row r="18" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="19" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4014,23 +4018,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="28"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="32"/>
-      <c r="I2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="6">
@@ -4086,44 +4090,44 @@
       <c r="D13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
     </row>
     <row r="14" spans="3:9" ht="48" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="3:9" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
     </row>
     <row r="16" spans="3:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5129,7 +5133,7 @@
   <dimension ref="C1:I1000"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5141,14 +5145,14 @@
   <sheetData>
     <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="28"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H3" s="32"/>
-      <c r="I3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -5184,11 +5188,11 @@
       <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C12" s="8"/>
@@ -5196,11 +5200,11 @@
         <f>SUM(C6:C8)</f>
         <v>60</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="39"/>
     </row>
     <row r="13" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C13" s="8"/>
@@ -5208,39 +5212,49 @@
         <f>SUM(C6:C7,C8)</f>
         <v>60</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="15" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="16" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="17" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D17" s="47" t="s">
+    <row r="17" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D17" s="26" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D18" s="48">
+      <c r="H17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D18" s="27">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="21" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="29" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="30" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+      <c r="H18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H19">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="4:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6237,23 +6251,23 @@
   <sheetData>
     <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="28"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H3" s="32"/>
-      <c r="I3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="7" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="39"/>
     </row>
     <row r="8" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C8" s="6" t="s">
@@ -6296,38 +6310,38 @@
       <c r="D14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="3:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" spans="3:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="19" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7343,14 +7357,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="32"/>
-      <c r="H2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7409,10 +7423,10 @@
       <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
@@ -7422,26 +7436,26 @@
         <f>SUMIFS(C6:C9,C6:C9,"&gt;100",C6:C9,"&lt;500")</f>
         <v>600</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="2:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="37"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="37"/>
+      <c r="E14" s="39"/>
     </row>
     <row r="15" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="16" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8460,15 +8474,15 @@
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="14"/>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="14"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="14"/>
@@ -11528,10 +11542,10 @@
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="28"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C2" s="14"/>
@@ -11539,8 +11553,8 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="14"/>
@@ -11641,47 +11655,47 @@
       <c r="D13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14" spans="3:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C14" s="18"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="3:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" s="18"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" spans="3:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C16" s="18"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" spans="3:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C17" s="18"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C18" s="14"/>
@@ -18583,7 +18597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -18595,14 +18609,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="32"/>
-      <c r="H2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -18665,38 +18679,38 @@
       <c r="C13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
     </row>
     <row r="14" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -19700,7 +19714,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C1:I1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
@@ -19711,14 +19727,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="28"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="32"/>
-      <c r="I2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -19761,47 +19777,47 @@
       <c r="D15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C16" s="18"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" spans="3:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C17" s="18"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="3:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C18" s="18"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" spans="3:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C19" s="18"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="39"/>
     </row>
     <row r="20" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="21" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -20794,8 +20810,8 @@
     <mergeCell ref="E18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -20814,23 +20830,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="32"/>
-      <c r="H2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="39"/>
     </row>
     <row r="7" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="6" t="s">
@@ -20882,38 +20898,38 @@
       <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="20" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>